<commit_message>
about to use an enum for column names
</commit_message>
<xml_diff>
--- a/override.xlsx
+++ b/override.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t xml:space="preserve">Rules are processed in order by the finance app</t>
   </si>
@@ -64,6 +64,18 @@
     <t xml:space="preserve">$market=(.*)</t>
   </si>
   <si>
+    <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${ticker}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ticker=(.*)</t>
+  </si>
+  <si>
     <t xml:space="preserve">PickType</t>
   </si>
   <si>
@@ -88,18 +100,12 @@
     <t xml:space="preserve">$picktype=(.*)</t>
   </si>
   <si>
-    <t xml:space="preserve">JoinManyDesc</t>
+    <t xml:space="preserve">PickDesc</t>
   </si>
   <si>
     <t xml:space="preserve">${picktype}:${ticker}</t>
   </si>
   <si>
-    <t xml:space="preserve">Ticker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$ticker=(.*)</t>
-  </si>
-  <si>
     <t xml:space="preserve">$ex=(.*)</t>
   </si>
   <si>
@@ -116,6 +122,30 @@
   </si>
   <si>
     <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$=NYSE|NASDAQ|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$=Eurex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$=SBF|EPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDFd</t>
   </si>
 </sst>
 </file>
@@ -231,13 +261,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
@@ -307,101 +337,104 @@
       <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="0" t="n">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="0" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="0" t="n">
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="0" t="n">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="0" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,16 +442,16 @@
         <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,18 +459,104 @@
         <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>